<commit_message>
yeah. forgot to commit this changes...
</commit_message>
<xml_diff>
--- a/data-raw/datasets_MSUpeers-WMUpeers.xlsx
+++ b/data-raw/datasets_MSUpeers-WMUpeers.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/emilioxavieresposito/GitHub/theHUB/data-raw/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{297B7ADB-427A-D048-8F75-89846E664C25}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8809AEFD-CC90-4A4E-A4A7-AA026FB1E417}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="8660" yWindow="1860" windowWidth="35000" windowHeight="24980" xr2:uid="{88C0ADCA-6F07-6A4E-8FA9-4CD01068784F}"/>
   </bookViews>
@@ -2835,10 +2835,10 @@
   <dimension ref="A1:T93"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="140" zoomScaleNormal="140" workbookViewId="0">
-      <pane xSplit="1" ySplit="1" topLeftCell="B50" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="1" ySplit="1" topLeftCell="B2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="H84" sqref="H84"/>
+      <selection pane="bottomRight" activeCell="I28" sqref="I28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -3419,28 +3419,28 @@
     </row>
     <row r="10" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A10" s="4" t="s">
-        <v>78</v>
+        <v>176</v>
       </c>
       <c r="B10" s="4" t="s">
-        <v>79</v>
+        <v>177</v>
       </c>
       <c r="C10" s="4">
-        <v>145637</v>
+        <v>110662</v>
       </c>
       <c r="D10" s="5" t="s">
-        <v>80</v>
+        <v>178</v>
       </c>
       <c r="E10" s="5" t="s">
-        <v>81</v>
+        <v>179</v>
       </c>
       <c r="F10" s="4" t="s">
-        <v>82</v>
+        <v>180</v>
       </c>
       <c r="G10" s="4" t="s">
-        <v>38</v>
+        <v>162</v>
       </c>
       <c r="H10" s="5" t="s">
-        <v>83</v>
+        <v>181</v>
       </c>
       <c r="I10" s="4">
         <v>8</v>
@@ -3449,7 +3449,7 @@
         <v>1</v>
       </c>
       <c r="K10" s="4" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="L10" s="4" t="b">
         <v>0</v>
@@ -3458,7 +3458,7 @@
         <v>1</v>
       </c>
       <c r="N10" s="4" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="O10" s="4" t="b">
         <v>1</v>
@@ -3473,36 +3473,36 @@
         <v>1</v>
       </c>
       <c r="S10" s="6" t="s">
-        <v>84</v>
+        <v>701</v>
       </c>
       <c r="T10" s="6" t="s">
-        <v>85</v>
+        <v>702</v>
       </c>
     </row>
     <row r="11" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A11" s="4" t="s">
-        <v>86</v>
+        <v>78</v>
       </c>
       <c r="B11" s="4" t="s">
-        <v>87</v>
+        <v>79</v>
       </c>
       <c r="C11" s="4">
-        <v>153658</v>
+        <v>145637</v>
       </c>
       <c r="D11" s="5" t="s">
-        <v>88</v>
+        <v>80</v>
       </c>
       <c r="E11" s="5" t="s">
-        <v>89</v>
+        <v>81</v>
       </c>
       <c r="F11" s="4" t="s">
-        <v>90</v>
+        <v>82</v>
       </c>
       <c r="G11" s="4" t="s">
-        <v>91</v>
+        <v>38</v>
       </c>
       <c r="H11" s="5" t="s">
-        <v>92</v>
+        <v>83</v>
       </c>
       <c r="I11" s="4">
         <v>9</v>
@@ -3520,7 +3520,7 @@
         <v>1</v>
       </c>
       <c r="N11" s="4" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="O11" s="4" t="b">
         <v>1</v>
@@ -3535,36 +3535,36 @@
         <v>1</v>
       </c>
       <c r="S11" s="6" t="s">
-        <v>93</v>
+        <v>84</v>
       </c>
       <c r="T11" s="6" t="s">
-        <v>68</v>
+        <v>85</v>
       </c>
     </row>
     <row r="12" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A12" s="4" t="s">
-        <v>94</v>
+        <v>86</v>
       </c>
       <c r="B12" s="4" t="s">
-        <v>95</v>
+        <v>87</v>
       </c>
       <c r="C12" s="4">
-        <v>163286</v>
+        <v>153658</v>
       </c>
       <c r="D12" s="5" t="s">
-        <v>96</v>
+        <v>88</v>
       </c>
       <c r="E12" s="5" t="s">
-        <v>97</v>
+        <v>89</v>
       </c>
       <c r="F12" s="4" t="s">
-        <v>98</v>
+        <v>90</v>
       </c>
       <c r="G12" s="4" t="s">
-        <v>99</v>
+        <v>91</v>
       </c>
       <c r="H12" s="5" t="s">
-        <v>100</v>
+        <v>92</v>
       </c>
       <c r="I12" s="4">
         <v>10</v>
@@ -3582,7 +3582,7 @@
         <v>1</v>
       </c>
       <c r="N12" s="4" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="O12" s="4" t="b">
         <v>1</v>
@@ -3597,36 +3597,36 @@
         <v>1</v>
       </c>
       <c r="S12" s="6" t="s">
-        <v>101</v>
+        <v>93</v>
       </c>
       <c r="T12" s="6" t="s">
-        <v>102</v>
+        <v>68</v>
       </c>
     </row>
     <row r="13" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A13" s="4" t="s">
-        <v>103</v>
+        <v>94</v>
       </c>
       <c r="B13" s="4" t="s">
-        <v>104</v>
+        <v>95</v>
       </c>
       <c r="C13" s="4">
-        <v>170976</v>
+        <v>163286</v>
       </c>
       <c r="D13" s="5" t="s">
-        <v>105</v>
+        <v>96</v>
       </c>
       <c r="E13" s="5" t="s">
-        <v>106</v>
+        <v>97</v>
       </c>
       <c r="F13" s="4" t="s">
-        <v>107</v>
+        <v>98</v>
       </c>
       <c r="G13" s="4" t="s">
-        <v>29</v>
+        <v>99</v>
       </c>
       <c r="H13" s="5" t="s">
-        <v>108</v>
+        <v>100</v>
       </c>
       <c r="I13" s="4">
         <v>11</v>
@@ -3644,13 +3644,13 @@
         <v>1</v>
       </c>
       <c r="N13" s="4" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="O13" s="4" t="b">
         <v>1</v>
       </c>
       <c r="P13" s="4" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="Q13" s="4" t="b">
         <v>0</v>
@@ -3659,36 +3659,36 @@
         <v>1</v>
       </c>
       <c r="S13" s="6" t="s">
-        <v>109</v>
+        <v>101</v>
       </c>
       <c r="T13" s="6" t="s">
-        <v>110</v>
+        <v>102</v>
       </c>
     </row>
     <row r="14" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A14" s="4" t="s">
-        <v>111</v>
+        <v>103</v>
       </c>
       <c r="B14" s="4" t="s">
-        <v>112</v>
+        <v>104</v>
       </c>
       <c r="C14" s="4">
-        <v>174066</v>
+        <v>170976</v>
       </c>
       <c r="D14" s="5" t="s">
-        <v>113</v>
+        <v>105</v>
       </c>
       <c r="E14" s="5" t="s">
-        <v>114</v>
+        <v>106</v>
       </c>
       <c r="F14" s="4" t="s">
-        <v>115</v>
+        <v>107</v>
       </c>
       <c r="G14" s="4" t="s">
-        <v>116</v>
+        <v>29</v>
       </c>
       <c r="H14" s="5" t="s">
-        <v>117</v>
+        <v>108</v>
       </c>
       <c r="I14" s="4">
         <v>12</v>
@@ -3706,13 +3706,13 @@
         <v>1</v>
       </c>
       <c r="N14" s="4" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="O14" s="4" t="b">
         <v>1</v>
       </c>
       <c r="P14" s="4" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="Q14" s="4" t="b">
         <v>0</v>
@@ -3721,36 +3721,36 @@
         <v>1</v>
       </c>
       <c r="S14" s="6" t="s">
-        <v>118</v>
+        <v>109</v>
       </c>
       <c r="T14" s="6" t="s">
-        <v>119</v>
+        <v>110</v>
       </c>
     </row>
     <row r="15" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A15" s="4" t="s">
-        <v>120</v>
+        <v>111</v>
       </c>
       <c r="B15" s="4" t="s">
-        <v>121</v>
+        <v>112</v>
       </c>
       <c r="C15" s="4">
-        <v>181464</v>
+        <v>174066</v>
       </c>
       <c r="D15" s="5" t="s">
-        <v>122</v>
+        <v>113</v>
       </c>
       <c r="E15" s="5" t="s">
-        <v>123</v>
+        <v>114</v>
       </c>
       <c r="F15" s="4" t="s">
-        <v>124</v>
+        <v>115</v>
       </c>
       <c r="G15" s="4" t="s">
-        <v>125</v>
+        <v>116</v>
       </c>
       <c r="H15" s="5" t="s">
-        <v>126</v>
+        <v>117</v>
       </c>
       <c r="I15" s="4">
         <v>13</v>
@@ -3771,7 +3771,7 @@
         <v>1</v>
       </c>
       <c r="O15" s="4" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="P15" s="4" t="b">
         <v>0</v>
@@ -3783,36 +3783,36 @@
         <v>1</v>
       </c>
       <c r="S15" s="6" t="s">
-        <v>127</v>
+        <v>118</v>
       </c>
       <c r="T15" s="6" t="s">
-        <v>128</v>
+        <v>119</v>
       </c>
     </row>
     <row r="16" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A16" s="4" t="s">
-        <v>129</v>
+        <v>120</v>
       </c>
       <c r="B16" s="4" t="s">
-        <v>130</v>
+        <v>121</v>
       </c>
       <c r="C16" s="4">
-        <v>240444</v>
+        <v>181464</v>
       </c>
       <c r="D16" s="5" t="s">
-        <v>131</v>
+        <v>122</v>
       </c>
       <c r="E16" s="5" t="s">
-        <v>132</v>
+        <v>123</v>
       </c>
       <c r="F16" s="4" t="s">
-        <v>133</v>
+        <v>124</v>
       </c>
       <c r="G16" s="4" t="s">
-        <v>134</v>
+        <v>125</v>
       </c>
       <c r="H16" s="5" t="s">
-        <v>135</v>
+        <v>126</v>
       </c>
       <c r="I16" s="4">
         <v>14</v>
@@ -3833,7 +3833,7 @@
         <v>1</v>
       </c>
       <c r="O16" s="4" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="P16" s="4" t="b">
         <v>0</v>
@@ -3845,42 +3845,42 @@
         <v>1</v>
       </c>
       <c r="S16" s="6" t="s">
-        <v>136</v>
+        <v>127</v>
       </c>
       <c r="T16" s="6" t="s">
-        <v>59</v>
+        <v>128</v>
       </c>
     </row>
     <row r="17" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A17" s="4" t="s">
-        <v>519</v>
+        <v>247</v>
       </c>
       <c r="B17" s="4" t="s">
-        <v>520</v>
+        <v>248</v>
       </c>
       <c r="C17" s="4">
-        <v>104151</v>
+        <v>209551</v>
       </c>
       <c r="D17" s="5" t="s">
-        <v>521</v>
+        <v>249</v>
       </c>
       <c r="E17" s="5" t="s">
-        <v>522</v>
+        <v>250</v>
       </c>
       <c r="F17" s="4" t="s">
-        <v>523</v>
+        <v>251</v>
       </c>
       <c r="G17" s="4" t="s">
-        <v>155</v>
+        <v>252</v>
       </c>
       <c r="H17" s="5" t="s">
-        <v>524</v>
+        <v>253</v>
       </c>
       <c r="I17" s="4">
         <v>15</v>
       </c>
       <c r="J17" s="4" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="K17" s="4" t="b">
         <v>1</v>
@@ -3895,7 +3895,7 @@
         <v>0</v>
       </c>
       <c r="O17" s="4" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="P17" s="4" t="b">
         <v>0</v>
@@ -3907,42 +3907,42 @@
         <v>1</v>
       </c>
       <c r="S17" s="6" t="s">
-        <v>695</v>
+        <v>704</v>
       </c>
       <c r="T17" s="6" t="s">
-        <v>696</v>
+        <v>705</v>
       </c>
     </row>
     <row r="18" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A18" s="4" t="s">
-        <v>150</v>
+        <v>525</v>
       </c>
       <c r="B18" s="4" t="s">
-        <v>151</v>
+        <v>526</v>
       </c>
       <c r="C18" s="4">
-        <v>104179</v>
+        <v>123961</v>
       </c>
       <c r="D18" s="5" t="s">
-        <v>152</v>
+        <v>527</v>
       </c>
       <c r="E18" s="5" t="s">
-        <v>153</v>
+        <v>528</v>
       </c>
       <c r="F18" s="4" t="s">
-        <v>154</v>
+        <v>180</v>
       </c>
       <c r="G18" s="4" t="s">
-        <v>155</v>
+        <v>162</v>
       </c>
       <c r="H18" s="5" t="s">
-        <v>156</v>
+        <v>529</v>
       </c>
       <c r="I18" s="4">
         <v>16</v>
       </c>
       <c r="J18" s="4" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="K18" s="4" t="b">
         <v>1</v>
@@ -3951,10 +3951,10 @@
         <v>0</v>
       </c>
       <c r="M18" s="4" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="N18" s="4" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="O18" s="4" t="b">
         <v>1</v>
@@ -3969,42 +3969,42 @@
         <v>1</v>
       </c>
       <c r="S18" s="6" t="s">
-        <v>697</v>
+        <v>23</v>
       </c>
       <c r="T18" s="6" t="s">
-        <v>698</v>
+        <v>707</v>
       </c>
     </row>
     <row r="19" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A19" s="4" t="s">
-        <v>157</v>
+        <v>273</v>
       </c>
       <c r="B19" s="4" t="s">
-        <v>158</v>
+        <v>274</v>
       </c>
       <c r="C19" s="4">
-        <v>110635</v>
+        <v>236948</v>
       </c>
       <c r="D19" s="5" t="s">
-        <v>159</v>
+        <v>275</v>
       </c>
       <c r="E19" s="5" t="s">
-        <v>160</v>
+        <v>276</v>
       </c>
       <c r="F19" s="4" t="s">
-        <v>161</v>
+        <v>277</v>
       </c>
       <c r="G19" s="4" t="s">
-        <v>162</v>
+        <v>278</v>
       </c>
       <c r="H19" s="5" t="s">
-        <v>163</v>
+        <v>279</v>
       </c>
       <c r="I19" s="4">
         <v>17</v>
       </c>
       <c r="J19" s="4" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="K19" s="4" t="b">
         <v>1</v>
@@ -4016,7 +4016,7 @@
         <v>1</v>
       </c>
       <c r="N19" s="4" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="O19" s="4" t="b">
         <v>1</v>
@@ -4031,45 +4031,45 @@
         <v>1</v>
       </c>
       <c r="S19" s="6" t="s">
-        <v>699</v>
+        <v>693</v>
       </c>
       <c r="T19" s="6" t="s">
-        <v>700</v>
+        <v>694</v>
       </c>
     </row>
     <row r="20" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A20" s="4" t="s">
-        <v>176</v>
+        <v>129</v>
       </c>
       <c r="B20" s="4" t="s">
-        <v>177</v>
+        <v>130</v>
       </c>
       <c r="C20" s="4">
-        <v>110662</v>
+        <v>240444</v>
       </c>
       <c r="D20" s="5" t="s">
-        <v>178</v>
+        <v>131</v>
       </c>
       <c r="E20" s="5" t="s">
-        <v>179</v>
+        <v>132</v>
       </c>
       <c r="F20" s="4" t="s">
-        <v>180</v>
+        <v>133</v>
       </c>
       <c r="G20" s="4" t="s">
-        <v>162</v>
+        <v>134</v>
       </c>
       <c r="H20" s="5" t="s">
-        <v>181</v>
+        <v>135</v>
       </c>
       <c r="I20" s="4">
         <v>18</v>
       </c>
       <c r="J20" s="4" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="K20" s="4" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="L20" s="4" t="b">
         <v>0</v>
@@ -4078,7 +4078,7 @@
         <v>1</v>
       </c>
       <c r="N20" s="4" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="O20" s="4" t="b">
         <v>1</v>
@@ -4093,36 +4093,36 @@
         <v>1</v>
       </c>
       <c r="S20" s="6" t="s">
-        <v>701</v>
+        <v>136</v>
       </c>
       <c r="T20" s="6" t="s">
-        <v>702</v>
+        <v>59</v>
       </c>
     </row>
     <row r="21" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A21" s="4" t="s">
-        <v>226</v>
+        <v>519</v>
       </c>
       <c r="B21" s="4" t="s">
-        <v>227</v>
+        <v>520</v>
       </c>
       <c r="C21" s="4">
-        <v>126614</v>
+        <v>104151</v>
       </c>
       <c r="D21" s="5" t="s">
-        <v>228</v>
+        <v>521</v>
       </c>
       <c r="E21" s="5" t="s">
-        <v>229</v>
+        <v>522</v>
       </c>
       <c r="F21" s="4" t="s">
-        <v>230</v>
+        <v>523</v>
       </c>
       <c r="G21" s="4" t="s">
-        <v>231</v>
+        <v>155</v>
       </c>
       <c r="H21" s="5" t="s">
-        <v>232</v>
+        <v>524</v>
       </c>
       <c r="I21" s="4">
         <v>19</v>
@@ -4143,7 +4143,7 @@
         <v>0</v>
       </c>
       <c r="O21" s="4" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="P21" s="4" t="b">
         <v>0</v>
@@ -4155,36 +4155,36 @@
         <v>1</v>
       </c>
       <c r="S21" s="6" t="s">
-        <v>703</v>
+        <v>695</v>
       </c>
       <c r="T21" s="6" t="s">
-        <v>68</v>
+        <v>696</v>
       </c>
     </row>
     <row r="22" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A22" s="4" t="s">
-        <v>247</v>
+        <v>150</v>
       </c>
       <c r="B22" s="4" t="s">
-        <v>248</v>
+        <v>151</v>
       </c>
       <c r="C22" s="4">
-        <v>209551</v>
+        <v>104179</v>
       </c>
       <c r="D22" s="5" t="s">
-        <v>249</v>
+        <v>152</v>
       </c>
       <c r="E22" s="5" t="s">
-        <v>250</v>
+        <v>153</v>
       </c>
       <c r="F22" s="4" t="s">
-        <v>251</v>
+        <v>154</v>
       </c>
       <c r="G22" s="4" t="s">
-        <v>252</v>
+        <v>155</v>
       </c>
       <c r="H22" s="5" t="s">
-        <v>253</v>
+        <v>156</v>
       </c>
       <c r="I22" s="4">
         <v>20</v>
@@ -4202,7 +4202,7 @@
         <v>1</v>
       </c>
       <c r="N22" s="4" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="O22" s="4" t="b">
         <v>1</v>
@@ -4217,36 +4217,36 @@
         <v>1</v>
       </c>
       <c r="S22" s="6" t="s">
-        <v>704</v>
+        <v>697</v>
       </c>
       <c r="T22" s="6" t="s">
-        <v>705</v>
+        <v>698</v>
       </c>
     </row>
     <row r="23" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A23" s="4" t="s">
-        <v>574</v>
+        <v>157</v>
       </c>
       <c r="B23" s="4" t="s">
-        <v>581</v>
+        <v>158</v>
       </c>
       <c r="C23" s="4">
-        <v>209542</v>
+        <v>110635</v>
       </c>
       <c r="D23" s="5" t="s">
-        <v>616</v>
+        <v>159</v>
       </c>
       <c r="E23" s="5" t="s">
-        <v>617</v>
+        <v>160</v>
       </c>
       <c r="F23" s="4" t="s">
-        <v>618</v>
+        <v>161</v>
       </c>
       <c r="G23" s="4" t="s">
-        <v>252</v>
+        <v>162</v>
       </c>
       <c r="H23" s="5" t="s">
-        <v>619</v>
+        <v>163</v>
       </c>
       <c r="I23" s="4">
         <v>21</v>
@@ -4267,7 +4267,7 @@
         <v>1</v>
       </c>
       <c r="O23" s="4" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="P23" s="4" t="b">
         <v>0</v>
@@ -4279,36 +4279,36 @@
         <v>1</v>
       </c>
       <c r="S23" s="6" t="s">
-        <v>706</v>
+        <v>699</v>
       </c>
       <c r="T23" s="6" t="s">
-        <v>68</v>
+        <v>700</v>
       </c>
     </row>
     <row r="24" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A24" s="4" t="s">
-        <v>525</v>
+        <v>226</v>
       </c>
       <c r="B24" s="4" t="s">
-        <v>526</v>
+        <v>227</v>
       </c>
       <c r="C24" s="4">
-        <v>123961</v>
+        <v>126614</v>
       </c>
       <c r="D24" s="5" t="s">
-        <v>527</v>
+        <v>228</v>
       </c>
       <c r="E24" s="5" t="s">
-        <v>528</v>
+        <v>229</v>
       </c>
       <c r="F24" s="4" t="s">
-        <v>180</v>
+        <v>230</v>
       </c>
       <c r="G24" s="4" t="s">
-        <v>162</v>
+        <v>231</v>
       </c>
       <c r="H24" s="5" t="s">
-        <v>529</v>
+        <v>232</v>
       </c>
       <c r="I24" s="4">
         <v>22</v>
@@ -4323,7 +4323,7 @@
         <v>0</v>
       </c>
       <c r="M24" s="4" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="N24" s="4" t="b">
         <v>0</v>
@@ -4341,36 +4341,36 @@
         <v>1</v>
       </c>
       <c r="S24" s="6" t="s">
-        <v>23</v>
+        <v>703</v>
       </c>
       <c r="T24" s="6" t="s">
-        <v>707</v>
+        <v>68</v>
       </c>
     </row>
     <row r="25" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A25" s="4" t="s">
-        <v>575</v>
+        <v>574</v>
       </c>
       <c r="B25" s="4" t="s">
-        <v>580</v>
+        <v>581</v>
       </c>
       <c r="C25" s="4">
-        <v>243744</v>
+        <v>209542</v>
       </c>
       <c r="D25" s="5" t="s">
-        <v>620</v>
+        <v>616</v>
       </c>
       <c r="E25" s="5" t="s">
-        <v>621</v>
+        <v>617</v>
       </c>
       <c r="F25" s="4" t="s">
-        <v>580</v>
+        <v>618</v>
       </c>
       <c r="G25" s="4" t="s">
-        <v>162</v>
+        <v>252</v>
       </c>
       <c r="H25" s="5" t="s">
-        <v>622</v>
+        <v>619</v>
       </c>
       <c r="I25" s="4">
         <v>23</v>
@@ -4385,13 +4385,13 @@
         <v>0</v>
       </c>
       <c r="M25" s="4" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="N25" s="4" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="O25" s="4" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="P25" s="4" t="b">
         <v>0</v>
@@ -4403,36 +4403,36 @@
         <v>1</v>
       </c>
       <c r="S25" s="6" t="s">
-        <v>708</v>
+        <v>706</v>
       </c>
       <c r="T25" s="6" t="s">
-        <v>32</v>
+        <v>68</v>
       </c>
     </row>
     <row r="26" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A26" s="4" t="s">
-        <v>576</v>
+        <v>575</v>
       </c>
       <c r="B26" s="4" t="s">
-        <v>579</v>
-      </c>
-      <c r="C26" s="6">
-        <v>230764</v>
-      </c>
-      <c r="D26" s="7" t="s">
-        <v>623</v>
-      </c>
-      <c r="E26" s="7" t="s">
-        <v>624</v>
-      </c>
-      <c r="F26" s="6" t="s">
-        <v>625</v>
+        <v>580</v>
+      </c>
+      <c r="C26" s="4">
+        <v>243744</v>
+      </c>
+      <c r="D26" s="5" t="s">
+        <v>620</v>
+      </c>
+      <c r="E26" s="5" t="s">
+        <v>621</v>
+      </c>
+      <c r="F26" s="4" t="s">
+        <v>580</v>
       </c>
       <c r="G26" s="4" t="s">
-        <v>626</v>
-      </c>
-      <c r="H26" s="7" t="s">
-        <v>627</v>
+        <v>162</v>
+      </c>
+      <c r="H26" s="5" t="s">
+        <v>622</v>
       </c>
       <c r="I26" s="4">
         <v>24</v>
@@ -4447,7 +4447,7 @@
         <v>0</v>
       </c>
       <c r="M26" s="4" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="N26" s="4" t="b">
         <v>0</v>
@@ -4465,36 +4465,36 @@
         <v>1</v>
       </c>
       <c r="S26" s="6" t="s">
-        <v>709</v>
+        <v>708</v>
       </c>
       <c r="T26" s="6" t="s">
-        <v>68</v>
+        <v>32</v>
       </c>
     </row>
     <row r="27" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A27" s="4" t="s">
-        <v>273</v>
+        <v>576</v>
       </c>
       <c r="B27" s="4" t="s">
-        <v>274</v>
-      </c>
-      <c r="C27" s="4">
-        <v>236948</v>
-      </c>
-      <c r="D27" s="5" t="s">
-        <v>275</v>
-      </c>
-      <c r="E27" s="5" t="s">
-        <v>276</v>
-      </c>
-      <c r="F27" s="4" t="s">
-        <v>277</v>
+        <v>579</v>
+      </c>
+      <c r="C27" s="6">
+        <v>230764</v>
+      </c>
+      <c r="D27" s="7" t="s">
+        <v>623</v>
+      </c>
+      <c r="E27" s="7" t="s">
+        <v>624</v>
+      </c>
+      <c r="F27" s="6" t="s">
+        <v>625</v>
       </c>
       <c r="G27" s="4" t="s">
-        <v>278</v>
-      </c>
-      <c r="H27" s="5" t="s">
-        <v>279</v>
+        <v>626</v>
+      </c>
+      <c r="H27" s="7" t="s">
+        <v>627</v>
       </c>
       <c r="I27" s="4">
         <v>25</v>
@@ -4527,10 +4527,10 @@
         <v>1</v>
       </c>
       <c r="S27" s="6" t="s">
-        <v>693</v>
+        <v>709</v>
       </c>
       <c r="T27" s="6" t="s">
-        <v>694</v>
+        <v>68</v>
       </c>
     </row>
     <row r="28" spans="1:20" x14ac:dyDescent="0.2">

</xml_diff>